<commit_message>
Fixed duplicate "2019" data values
</commit_message>
<xml_diff>
--- a/observeddata/Ebola_Incidence_Data_4zones.xlsx
+++ b/observeddata/Ebola_Incidence_Data_4zones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twhit957\Desktop\spatialEpisim\observeddata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cupcake\Documents\MRU\Year 4\Winter\Senior Project\spatialEpisim\observeddata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90020B66-38E8-41AD-9D96-E473CECED85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80E6EB4-077B-4A20-9EF9-DEC8DBC8C64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Incidence" sheetId="1" r:id="rId1"/>
@@ -162,9 +162,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -202,7 +202,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -308,7 +308,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -450,7 +450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,7 +467,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>43682</v>
+        <v>43317</v>
       </c>
       <c r="C2" s="2">
         <v>34</v>
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>43689</v>
+        <v>43324</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -545,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>43697</v>
+        <v>43332</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -565,7 +565,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>43703</v>
+        <v>43338</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
@@ -585,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>43710</v>
+        <v>43345</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>
@@ -625,7 +625,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>43724</v>
+        <v>43359</v>
       </c>
       <c r="C8" s="2">
         <v>5</v>
@@ -645,7 +645,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>43731</v>
+        <v>43366</v>
       </c>
       <c r="C9" s="2">
         <v>4</v>
@@ -665,7 +665,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>43740</v>
+        <v>43375</v>
       </c>
       <c r="C10" s="2">
         <v>10</v>
@@ -685,7 +685,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>43745</v>
+        <v>43380</v>
       </c>
       <c r="C11" s="2">
         <v>14</v>
@@ -705,7 +705,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>43753</v>
+        <v>43388</v>
       </c>
       <c r="C12" s="2">
         <v>28</v>
@@ -725,7 +725,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>43759</v>
+        <v>43394</v>
       </c>
       <c r="C13" s="2">
         <v>19</v>
@@ -745,7 +745,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>43766</v>
+        <v>43401</v>
       </c>
       <c r="C14" s="2">
         <v>28</v>
@@ -765,7 +765,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>43773</v>
+        <v>43408</v>
       </c>
       <c r="C15" s="2">
         <v>16</v>
@@ -785,7 +785,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>43780</v>
+        <v>43415</v>
       </c>
       <c r="C16" s="2">
         <v>14</v>
@@ -805,7 +805,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>43788</v>
+        <v>43423</v>
       </c>
       <c r="C17" s="2">
         <v>14</v>
@@ -825,7 +825,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>43795</v>
+        <v>43430</v>
       </c>
       <c r="C18" s="2">
         <v>13</v>
@@ -845,7 +845,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>43802</v>
+        <v>43437</v>
       </c>
       <c r="C19" s="2">
         <v>8</v>
@@ -865,7 +865,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <v>43809</v>
+        <v>43444</v>
       </c>
       <c r="C20" s="2">
         <v>16</v>
@@ -885,7 +885,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>43815</v>
+        <v>43450</v>
       </c>
       <c r="C21" s="2">
         <v>3</v>
@@ -905,7 +905,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <v>43824</v>
+        <v>43459</v>
       </c>
       <c r="C22" s="2">
         <v>5</v>

</xml_diff>